<commit_message>
New Codes in excel
</commit_message>
<xml_diff>
--- a/True_Results.xlsx
+++ b/True_Results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\image project\STEP_ID-Scanner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3 Joe\2 Gam3a\Term 7\CMPS446 - Image Processing and Computer Vision\Project\STEP_Scanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05B5971-3E85-425C-BF3A-06D675A5687E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B4F049-D839-4A71-815C-30E57837F27F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{C1FA5F84-139F-4DC5-A2AD-8E0048BF87DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C1FA5F84-139F-4DC5-A2AD-8E0048BF87DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,12 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -164,9 +159,6 @@
     <t>احمد سامح صلاح مصيلحى</t>
   </si>
   <si>
-    <t>جنى ايمن وفائى محمد عيسى</t>
-  </si>
-  <si>
     <t>Student ID</t>
   </si>
   <si>
@@ -176,133 +168,37 @@
     <t>Daf3</t>
   </si>
   <si>
-    <t>ادهم احمد محمود ممدوح شبانة</t>
-  </si>
-  <si>
-    <t>14712020100041</t>
-  </si>
-  <si>
-    <t>14712022101214</t>
-  </si>
-  <si>
-    <t>14712022101495</t>
-  </si>
-  <si>
-    <t>14712022101358</t>
-  </si>
-  <si>
-    <t>14712022101524</t>
-  </si>
-  <si>
-    <t>14712522101392</t>
-  </si>
-  <si>
-    <t>14712022101329</t>
-  </si>
-  <si>
-    <t>14712022101620</t>
-  </si>
-  <si>
-    <t>14712022101322</t>
-  </si>
-  <si>
-    <t>14712022100089</t>
-  </si>
-  <si>
-    <t>14712022100080</t>
-  </si>
-  <si>
-    <t>14712022100036</t>
-  </si>
-  <si>
-    <t>14712022101553</t>
-  </si>
-  <si>
-    <t>1471202210078</t>
-  </si>
-  <si>
-    <t>14712022101079</t>
-  </si>
-  <si>
-    <t>14712022101373</t>
-  </si>
-  <si>
-    <t>14712022101354</t>
-  </si>
-  <si>
-    <t>14712022101537</t>
-  </si>
-  <si>
-    <t>14712022101624</t>
-  </si>
-  <si>
-    <t>14712022101610</t>
-  </si>
-  <si>
-    <t>14712022101262</t>
-  </si>
-  <si>
-    <t>14712020100046</t>
-  </si>
-  <si>
-    <t>14712023101281</t>
-  </si>
-  <si>
-    <t>14712019101774</t>
-  </si>
-  <si>
-    <t>14712023101223</t>
-  </si>
-  <si>
-    <t>14712022100623</t>
-  </si>
-  <si>
-    <t>14712022101552</t>
-  </si>
-  <si>
-    <t>14712021100205</t>
-  </si>
-  <si>
-    <t>14712023101217</t>
-  </si>
-  <si>
-    <t>14712021101550</t>
-  </si>
-  <si>
-    <t>14712021101455</t>
-  </si>
-  <si>
-    <t>14712021101553</t>
-  </si>
-  <si>
-    <t>14712018102167</t>
-  </si>
-  <si>
-    <t>14712021101568</t>
-  </si>
-  <si>
-    <t>14712023101286</t>
-  </si>
-  <si>
-    <t>14712023101060</t>
-  </si>
-  <si>
-    <t>14712022101505</t>
-  </si>
-  <si>
-    <t>14712022101338</t>
-  </si>
-  <si>
-    <t>14712023100148</t>
-  </si>
-  <si>
-    <t>14712022101628</t>
-  </si>
-  <si>
-    <t>14712021101365</t>
-  </si>
-  <si>
-    <t>14712022101345</t>
+    <t>يوسف احمد عفيفى منصور</t>
+  </si>
+  <si>
+    <t>(Obscured)</t>
+  </si>
+  <si>
+    <t>يحي محمود نصر محمود</t>
+  </si>
+  <si>
+    <t>محمد سامح صبحي حسن صبيح</t>
+  </si>
+  <si>
+    <t>جمانه تيمور محمد البكرى احمد محمد</t>
+  </si>
+  <si>
+    <t>عبدالله سمير عبد الموجود عسكر</t>
+  </si>
+  <si>
+    <t>حمزة احمد محمد منير الجوهري</t>
+  </si>
+  <si>
+    <t>لوجينا شوقي أحمد شحاته</t>
+  </si>
+  <si>
+    <t>احمد وائل محمد جويد نحيله</t>
+  </si>
+  <si>
+    <t>محمد هشام ابراهيم حسنين</t>
+  </si>
+  <si>
+    <t>يوسف عصام عبدالمنعم احمد منسي</t>
   </si>
 </sst>
 </file>
@@ -334,12 +230,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -392,22 +289,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,9 +327,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -467,7 +367,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -573,7 +473,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -715,7 +615,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -723,828 +623,794 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCAA91C-A1A6-447C-9C97-0B0A038DB89C}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="27.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>1200277</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>14712020100041</v>
       </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>1220175</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>14712022101252</v>
       </c>
-      <c r="E3">
-        <v>14712022101252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>1220165</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>14712022101214</v>
       </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>1220145</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>14712022101495</v>
       </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>1220237</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>14712022101358</v>
       </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>4230174</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>14712022101524</v>
       </c>
-      <c r="E7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>1220301</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>14712022101392</v>
       </c>
-      <c r="E8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>1220205</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>14712022101329</v>
       </c>
-      <c r="E9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>1220149</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>14712022101620</v>
       </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>1220319</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>14712022101322</v>
       </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>1220092</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>14712022100089</v>
       </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>1220188</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="5">
         <v>14712022100080</v>
       </c>
-      <c r="E13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>1220062</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>14712022100036</v>
       </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>4230189</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <v>14712022101553</v>
       </c>
-      <c r="E15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>4230160</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <v>14712022100643</v>
       </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>4230142</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5">
         <v>14712022101079</v>
       </c>
-      <c r="E17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <v>1220279</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <v>14712022101373</v>
       </c>
-      <c r="E18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="4">
         <v>1220256</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="5">
         <v>14712022101354</v>
       </c>
-      <c r="E19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>1220123</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="5">
         <v>14712022101537</v>
       </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>1220137</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="5">
         <v>14712022101624</v>
       </c>
-      <c r="E21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="4">
         <v>4230159</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="5">
         <v>14712022101610</v>
       </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <v>1220125</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="5">
         <v>14712022101262</v>
       </c>
-      <c r="E23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="4">
         <v>1200309</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="5">
         <v>14712020100046</v>
       </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="4">
         <v>4230189</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="5">
         <v>14712022101553</v>
       </c>
-      <c r="E25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1200883</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="3">
-        <v>1230157</v>
-      </c>
-      <c r="D26" s="4">
-        <v>14712023101281</v>
-      </c>
-      <c r="E26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="4">
         <v>1190533</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="5">
         <v>14712019101776</v>
       </c>
-      <c r="E27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="4">
         <v>1230165</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="5">
         <v>14712023101223</v>
       </c>
-      <c r="E28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="4">
         <v>1220003</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="5">
         <v>14712022100623</v>
       </c>
-      <c r="E29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="4">
         <v>1220121</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="5">
         <v>14712022101552</v>
       </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="4">
         <v>1210096</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="5">
         <v>14712021100205</v>
       </c>
-      <c r="E31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="4">
         <v>1230315</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="5">
         <v>14712023101217</v>
       </c>
-      <c r="E32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="4">
         <v>1210216</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="5">
         <v>14712021101550</v>
       </c>
-      <c r="E33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="4">
         <v>1210227</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="5">
         <v>14712021101455</v>
       </c>
-      <c r="E34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="4">
         <v>1230165</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="5">
         <v>14712023101223</v>
       </c>
-      <c r="E35" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="4">
         <v>1210235</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="5">
         <v>14712021101553</v>
       </c>
-      <c r="E36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="4">
         <v>1180568</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="5">
         <v>14712018102167</v>
       </c>
-      <c r="E37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="3">
-        <v>1210349</v>
-      </c>
-      <c r="D38" s="4">
-        <v>14712021101568</v>
-      </c>
-      <c r="E38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1200454</v>
+      </c>
+      <c r="D38" s="5">
+        <v>14712020101893</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="4">
         <v>1230196</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D39" s="5">
         <v>14712023101286</v>
       </c>
-      <c r="E39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="4">
         <v>1220279</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D40" s="5">
         <v>14712022101373</v>
       </c>
-      <c r="E40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="4">
         <v>1230030</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="5">
         <v>14712023101060</v>
       </c>
-      <c r="E41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="3">
-        <v>4230138</v>
-      </c>
-      <c r="D42" s="4">
-        <v>14712022101505</v>
-      </c>
-      <c r="E42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="4">
+        <v>1200460</v>
+      </c>
+      <c r="D42" s="5">
+        <v>14712020102030</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="4">
         <v>1220273</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D43" s="5">
         <v>14712022101338</v>
       </c>
-      <c r="E43" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="4">
         <v>1230144</v>
       </c>
-      <c r="D44" s="4">
+      <c r="D44" s="5">
         <v>14712023100148</v>
       </c>
-      <c r="E44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="4">
         <v>1220221</v>
       </c>
-      <c r="D45" s="4">
+      <c r="D45" s="5">
         <v>14712022101628</v>
       </c>
-      <c r="E45" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="4">
         <v>1210284</v>
       </c>
-      <c r="D46" s="4">
+      <c r="D46" s="5">
         <v>14712021101365</v>
       </c>
-      <c r="E46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="4">
         <v>1220229</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="5">
         <v>14712022101345</v>
       </c>
-      <c r="E47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="2"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="4">
+        <v>4230138</v>
+      </c>
+      <c r="D48" s="5">
+        <v>14712022101505</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="4">
+        <v>1220006</v>
+      </c>
+      <c r="D49" s="5">
+        <v>14712022100861</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1230204</v>
+      </c>
+      <c r="D50" s="5">
+        <v>14712023101193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="4">
+        <v>1220169</v>
+      </c>
+      <c r="D51" s="5">
+        <v>14712022101244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C52" s="4">
+        <v>1220138</v>
+      </c>
+      <c r="D52" s="5">
+        <v>14712022101562</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="4">
+        <v>1220162</v>
+      </c>
+      <c r="D53" s="5">
+        <v>14712022101210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="4">
+        <v>1220278</v>
+      </c>
+      <c r="D54" s="5">
+        <v>14712022101414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="4">
+        <v>1220090</v>
+      </c>
+      <c r="D55" s="5">
+        <v>14712022100101</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>